<commit_message>
Added %CVMatch in ExtractCVs.xaml file
</commit_message>
<xml_diff>
--- a/Data/ConfigurationSettings.xlsx
+++ b/Data/ConfigurationSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Ray\Ray PC Home\Raymond\Raymond Loh Wee Ping Resume\Race Academy\2021\Course Notes\RPA Projects\RPAJ01_JobMatchingForPlacements\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A54554-BA9D-4598-9868-9218961318D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D4F20A-534B-4311-942E-DB6EDFDFC2C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configurations" sheetId="2" r:id="rId1"/>
@@ -493,13 +493,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="34.58203125" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.75" customWidth="1"/>
     <col min="3" max="26" width="7.625" customWidth="1"/>
   </cols>
@@ -2214,7 +2214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA01E30-B860-426B-B662-508E3DC414F9}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>